<commit_message>
added comments and fixed the excel sheet
</commit_message>
<xml_diff>
--- a/src/main/resources/Clement Task.xlsx
+++ b/src/main/resources/Clement Task.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17766"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17830"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\HW Help\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\HW Help\MatrixSort\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -26,7 +26,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
-    <t>Find the following numbers in different unit test: 55, 35, 11, 2222 and 200000</t>
+    <t>Find the following numbers in different unit test: 5005, 1012, 6, 53</t>
   </si>
 </sst>
 </file>
@@ -69,7 +69,18 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -379,7 +390,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J13"/>
+  <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="K10" sqref="K10"/>
@@ -387,335 +398,405 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="10" max="10" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="9" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1">
         <v>1</v>
       </c>
       <c r="B1" s="1">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1">
         <v>4</v>
-      </c>
-      <c r="C1" s="1">
-        <v>5</v>
       </c>
       <c r="D1" s="1">
         <v>6</v>
       </c>
       <c r="E1" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F1" s="1">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="G1" s="1">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="H1" s="1">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="I1" s="1">
-        <v>100</v>
+        <v>26</v>
       </c>
       <c r="J1" s="1">
-        <v>1234</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+        <v>1000</v>
+      </c>
+      <c r="K1" s="1">
+        <v>1002</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>3</v>
       </c>
       <c r="B2" s="1">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C2" s="1">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D2" s="1">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="E2" s="1">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="F2" s="1">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="G2" s="1">
-        <v>16</v>
+        <v>34</v>
       </c>
       <c r="H2" s="1">
-        <v>17</v>
+        <v>42</v>
       </c>
       <c r="I2" s="1">
-        <v>111</v>
+        <v>62</v>
       </c>
       <c r="J2" s="1">
-        <v>2222</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+        <v>1004</v>
+      </c>
+      <c r="K2" s="1">
+        <v>1010</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>5</v>
       </c>
       <c r="B3" s="1">
+        <v>15</v>
+      </c>
+      <c r="C3" s="1">
+        <v>27</v>
+      </c>
+      <c r="D3" s="1">
+        <v>30</v>
+      </c>
+      <c r="E3" s="1">
+        <v>36</v>
+      </c>
+      <c r="F3" s="1">
+        <v>38</v>
+      </c>
+      <c r="G3" s="1">
+        <v>40</v>
+      </c>
+      <c r="H3" s="1">
+        <v>44</v>
+      </c>
+      <c r="I3" s="1">
+        <v>70</v>
+      </c>
+      <c r="J3" s="1">
+        <v>1012</v>
+      </c>
+      <c r="K3" s="1">
+        <v>1020</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>7</v>
+      </c>
+      <c r="B4" s="1">
+        <v>19</v>
+      </c>
+      <c r="C4" s="1">
+        <v>29</v>
+      </c>
+      <c r="D4" s="1">
+        <v>49</v>
+      </c>
+      <c r="E4" s="1">
+        <v>50</v>
+      </c>
+      <c r="F4" s="1">
+        <v>52</v>
+      </c>
+      <c r="G4" s="1">
+        <v>54</v>
+      </c>
+      <c r="H4" s="1">
+        <v>60</v>
+      </c>
+      <c r="I4" s="1">
+        <v>72</v>
+      </c>
+      <c r="J4" s="1">
+        <v>1040</v>
+      </c>
+      <c r="K4" s="1">
+        <v>1100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>9</v>
+      </c>
+      <c r="B5" s="1">
+        <v>21</v>
+      </c>
+      <c r="C5" s="1">
+        <v>35</v>
+      </c>
+      <c r="D5" s="1">
+        <v>55</v>
+      </c>
+      <c r="E5" s="1">
+        <v>69</v>
+      </c>
+      <c r="F5" s="1">
+        <v>74</v>
+      </c>
+      <c r="G5" s="1">
+        <v>78</v>
+      </c>
+      <c r="H5" s="1">
+        <v>80</v>
+      </c>
+      <c r="I5" s="1">
+        <v>90</v>
+      </c>
+      <c r="J5" s="1">
+        <v>1110</v>
+      </c>
+      <c r="K5" s="1">
+        <v>1150</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
         <v>11</v>
       </c>
-      <c r="C3" s="1">
-        <v>13</v>
-      </c>
-      <c r="D3" s="1">
-        <v>14</v>
-      </c>
-      <c r="E3" s="1">
-        <v>15</v>
-      </c>
-      <c r="F3" s="1">
-        <v>16</v>
-      </c>
-      <c r="G3" s="1">
+      <c r="B6" s="1">
+        <v>23</v>
+      </c>
+      <c r="C6" s="1">
+        <v>39</v>
+      </c>
+      <c r="D6" s="1">
+        <v>57</v>
+      </c>
+      <c r="E6" s="1">
+        <v>73</v>
+      </c>
+      <c r="F6" s="1">
+        <v>83</v>
+      </c>
+      <c r="G6" s="1">
+        <v>94</v>
+      </c>
+      <c r="H6" s="1">
+        <v>98</v>
+      </c>
+      <c r="I6" s="1">
+        <v>1018</v>
+      </c>
+      <c r="J6" s="1">
+        <v>1130</v>
+      </c>
+      <c r="K6" s="1">
+        <v>1180</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
         <v>17</v>
       </c>
-      <c r="H3" s="1">
-        <v>18</v>
-      </c>
-      <c r="I3" s="1">
-        <v>5445</v>
-      </c>
-      <c r="J3" s="1">
-        <v>60000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>6</v>
-      </c>
-      <c r="B4" s="1">
-        <v>15</v>
-      </c>
-      <c r="C4" s="1">
-        <v>16</v>
-      </c>
-      <c r="D4" s="1">
-        <v>17</v>
-      </c>
-      <c r="E4" s="1">
-        <v>18</v>
-      </c>
-      <c r="F4" s="1">
+      <c r="B7" s="1">
         <v>33</v>
       </c>
-      <c r="G4" s="1">
-        <v>55</v>
-      </c>
-      <c r="H4" s="1">
-        <v>77</v>
-      </c>
-      <c r="I4" s="1">
-        <v>10000</v>
-      </c>
-      <c r="J4" s="1">
-        <v>65666</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>8</v>
-      </c>
-      <c r="B5" s="1">
+      <c r="C7" s="1">
+        <v>43</v>
+      </c>
+      <c r="D7" s="1">
+        <v>61</v>
+      </c>
+      <c r="E7" s="1">
+        <v>75</v>
+      </c>
+      <c r="F7" s="1">
+        <v>85</v>
+      </c>
+      <c r="G7" s="1">
+        <v>97</v>
+      </c>
+      <c r="H7" s="1">
+        <v>100</v>
+      </c>
+      <c r="I7" s="1">
+        <v>1030</v>
+      </c>
+      <c r="J7" s="1">
+        <v>1140</v>
+      </c>
+      <c r="K7" s="1">
+        <v>1190</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
         <v>25</v>
       </c>
-      <c r="C5" s="1">
-        <v>30</v>
-      </c>
-      <c r="D5" s="1">
-        <v>31</v>
-      </c>
-      <c r="E5" s="1">
-        <v>32</v>
-      </c>
-      <c r="F5" s="1">
-        <v>35</v>
-      </c>
-      <c r="G5" s="1">
-        <v>70</v>
-      </c>
-      <c r="H5" s="1">
-        <v>90</v>
-      </c>
-      <c r="I5" s="1">
-        <v>15000</v>
-      </c>
-      <c r="J5" s="1">
-        <v>70000</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>9</v>
-      </c>
-      <c r="B6" s="1">
-        <v>28</v>
-      </c>
-      <c r="C6" s="1">
-        <v>33</v>
-      </c>
-      <c r="D6" s="1">
-        <v>34</v>
-      </c>
-      <c r="E6" s="1">
-        <v>35</v>
-      </c>
-      <c r="F6" s="1">
+      <c r="B8" s="1">
         <v>37</v>
       </c>
-      <c r="G6" s="1">
-        <v>80</v>
-      </c>
-      <c r="H6" s="1">
-        <v>100</v>
-      </c>
-      <c r="I6" s="1">
-        <v>20000</v>
-      </c>
-      <c r="J6" s="1">
-        <v>80000</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
-        <v>13</v>
-      </c>
-      <c r="B7" s="1">
-        <v>44</v>
-      </c>
-      <c r="C7" s="1">
-        <v>66</v>
-      </c>
-      <c r="D7" s="1">
+      <c r="C8" s="1">
+        <v>47</v>
+      </c>
+      <c r="D8" s="1">
+        <v>63</v>
+      </c>
+      <c r="E8" s="1">
+        <v>79</v>
+      </c>
+      <c r="F8" s="1">
+        <v>91</v>
+      </c>
+      <c r="G8" s="1">
+        <v>99</v>
+      </c>
+      <c r="H8" s="1">
+        <v>101</v>
+      </c>
+      <c r="I8" s="1">
+        <v>1050</v>
+      </c>
+      <c r="J8" s="1">
+        <v>1160</v>
+      </c>
+      <c r="K8" s="1">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>27</v>
+      </c>
+      <c r="B9" s="1">
+        <v>45</v>
+      </c>
+      <c r="C9" s="1">
+        <v>59</v>
+      </c>
+      <c r="D9" s="1">
         <v>67</v>
       </c>
-      <c r="E7" s="1">
-        <v>80</v>
-      </c>
-      <c r="F7" s="1">
-        <v>100</v>
-      </c>
-      <c r="G7" s="1">
-        <v>150</v>
-      </c>
-      <c r="H7" s="1">
-        <v>2000</v>
-      </c>
-      <c r="I7" s="1">
-        <v>100000</v>
-      </c>
-      <c r="J7" s="1">
-        <v>1000000</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
-        <v>26</v>
-      </c>
-      <c r="B8" s="1">
-        <v>55</v>
-      </c>
-      <c r="C8" s="1">
-        <v>67</v>
-      </c>
-      <c r="D8" s="1">
-        <v>80</v>
-      </c>
-      <c r="E8" s="1">
-        <v>90</v>
-      </c>
-      <c r="F8" s="1">
-        <v>111</v>
-      </c>
-      <c r="G8" s="1">
-        <v>555</v>
-      </c>
-      <c r="H8" s="1">
-        <v>30000</v>
-      </c>
-      <c r="I8" s="1">
-        <v>150000</v>
-      </c>
-      <c r="J8" s="1">
-        <v>2000000</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
-        <v>28</v>
-      </c>
-      <c r="B9" s="1">
-        <v>77</v>
-      </c>
-      <c r="C9" s="1">
-        <v>200</v>
-      </c>
-      <c r="D9" s="1">
-        <v>300</v>
-      </c>
       <c r="E9" s="1">
-        <v>400</v>
+        <v>81</v>
       </c>
       <c r="F9" s="1">
-        <v>500</v>
+        <v>93</v>
       </c>
       <c r="G9" s="1">
-        <v>600</v>
+        <v>1005</v>
       </c>
       <c r="H9" s="1">
-        <v>40000</v>
+        <v>1009</v>
       </c>
       <c r="I9" s="1">
-        <v>200000</v>
+        <v>3011</v>
       </c>
       <c r="J9" s="1">
-        <v>20000000</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+        <v>3000</v>
+      </c>
+      <c r="K9" s="1">
+        <v>8888</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>55</v>
+        <v>37</v>
       </c>
       <c r="B10" s="1">
-        <v>88</v>
+        <v>51</v>
       </c>
       <c r="C10" s="1">
-        <v>3000</v>
+        <v>1001</v>
       </c>
       <c r="D10" s="1">
-        <v>40000</v>
+        <v>1007</v>
       </c>
       <c r="E10" s="1">
-        <v>70000</v>
+        <v>1011</v>
       </c>
       <c r="F10" s="1">
-        <v>100000</v>
+        <v>1023</v>
       </c>
       <c r="G10" s="1">
-        <v>700000</v>
+        <v>1025</v>
       </c>
       <c r="H10" s="1">
-        <v>1000000</v>
+        <v>1027</v>
       </c>
       <c r="I10" s="1">
-        <v>5000000</v>
+        <v>4047</v>
       </c>
       <c r="J10" s="1">
-        <v>100000000</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+        <v>5005</v>
+      </c>
+      <c r="K10" s="1">
+        <v>12345678</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>41</v>
+      </c>
+      <c r="B11" s="1">
+        <v>53</v>
+      </c>
+      <c r="C11" s="1">
+        <v>1003</v>
+      </c>
+      <c r="D11" s="1">
+        <v>1117</v>
+      </c>
+      <c r="E11" s="1">
+        <v>1121</v>
+      </c>
+      <c r="F11" s="1">
+        <v>1123</v>
+      </c>
+      <c r="G11" s="1">
+        <v>1125</v>
+      </c>
+      <c r="H11" s="1">
+        <v>1135</v>
+      </c>
+      <c r="I11" s="1">
+        <v>9999</v>
+      </c>
+      <c r="J11" s="1">
+        <v>1111111</v>
+      </c>
+      <c r="K11" s="1">
+        <v>12345678912</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>0</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="A9">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>